<commit_message>
update: search by time query add: new admin dashboard navbar link new: person in charge update for OSC
</commit_message>
<xml_diff>
--- a/common/uploads/import_.xlsx
+++ b/common/uploads/import_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABAZAZILAH\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AACDD92-712F-4C02-B177-8CC407D885FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3156F50-2EAD-414E-8793-D505F25F6984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{18F5300B-07A7-4CB7-9271-079F2FF98243}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{18F5300B-07A7-4CB7-9271-079F2FF98243}"/>
   </bookViews>
   <sheets>
     <sheet name="KLM" sheetId="1" r:id="rId1"/>
@@ -1167,9 +1167,6 @@
     <t>USA</t>
   </si>
   <si>
-    <t>Kulliyyah of Engineering, Kulliyyah of Pharmacy, Kulliyyah of Languages and Management</t>
-  </si>
-  <si>
     <t xml:space="preserve">a)	to facilitate visits by individuals from each Party for the purpose of studying the other's educational system in order to develop cooperative mechanisms and to expand areas of cooperation;
 b)	to identify other areas of possible interest and collaboration; and
 c)	and to make faculty and students aware of the academic programs, research institutes, and educational resources of each other's institutions.
@@ -1196,6 +1193,9 @@
 Tel:        06-9742690
 Email:     mnzainiyah@iium.edu.my
 </t>
+  </si>
+  <si>
+    <t>Kulliyyah of Engineering</t>
   </si>
 </sst>
 </file>
@@ -1991,24 +1991,24 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" customWidth="1"/>
-    <col min="2" max="2" width="18.26953125" customWidth="1"/>
-    <col min="3" max="3" width="42.7265625" customWidth="1"/>
+    <col min="1" max="1" width="8.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="42.77734375" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="41" customWidth="1"/>
-    <col min="6" max="6" width="21.81640625" customWidth="1"/>
-    <col min="7" max="7" width="21.1796875" customWidth="1"/>
-    <col min="8" max="8" width="22.7265625" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" customWidth="1"/>
+    <col min="7" max="7" width="21.21875" customWidth="1"/>
+    <col min="8" max="8" width="22.77734375" customWidth="1"/>
     <col min="9" max="9" width="78" customWidth="1"/>
-    <col min="10" max="10" width="101.54296875" customWidth="1"/>
-    <col min="11" max="11" width="63.26953125" customWidth="1"/>
+    <col min="10" max="10" width="101.5546875" customWidth="1"/>
+    <col min="11" max="11" width="63.21875" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2744,7 +2744,7 @@
         <v>87</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F20" s="31">
         <v>2023</v>
@@ -2756,11 +2756,11 @@
         <v>46261</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J20" s="66"/>
       <c r="K20" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L20" s="9" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
update back end template update dashboard view new js global new sidebar.php update create, now allow only directed to oil application able to add ssm and company... update app assetes
</commit_message>
<xml_diff>
--- a/common/uploads/import_.xlsx
+++ b/common/uploads/import_.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABAZAZILAH\Downloads\moumoa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yamen\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A995FBFC-334A-47CE-9375-F2C5975DA93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2177302-46C5-4D0C-8E8B-2F75961EC6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{18F5300B-07A7-4CB7-9271-079F2FF98243}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18F5300B-07A7-4CB7-9271-079F2FF98243}"/>
   </bookViews>
   <sheets>
     <sheet name="KLM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KLM!$A$1:$L$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KLM!$A$1:$L$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="91">
   <si>
     <t>No</t>
   </si>
@@ -103,7 +103,6 @@
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Arial Narrow"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve">1)        4 students (Outbound Credited) Sem 1, 2017/2018
 2)        2 students (Outbound credited) Sem 2, 2017/2018
@@ -117,7 +116,6 @@
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Arial Narrow"/>
-        <family val="2"/>
       </rPr>
       <t>January - June 2022</t>
     </r>
@@ -126,7 +124,6 @@
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Arial Narrow"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - No activity reported
 </t>
@@ -137,7 +134,6 @@
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Arial Narrow"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve">July - December 2022 - </t>
     </r>
@@ -146,7 +142,6 @@
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Arial Narrow"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve">No activity reported
 </t>
@@ -157,7 +152,6 @@
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Arial Narrow"/>
-        <family val="2"/>
       </rPr>
       <t>Jan - June 2023</t>
     </r>
@@ -166,10 +160,22 @@
         <sz val="13"/>
         <color theme="1"/>
         <rFont val="Arial Narrow"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - 1 student exchange (Outbound credited) on 1 April - 20 September 2023</t>
     </r>
+  </si>
+  <si>
+    <t>Assoc. Prof. Dr. Mohd Azrul Azlen bin Abd Hamid
+Kulliyyah of Languages and Management
+International Islamic University Malaysia (IIUM) Pagoh Edu Hub
+KM 1, Jalan Panchor,
+84600, Pagoh, Muar,
+Johor Darul Takzim,
+Tel : 06 - 974 2606
+Email : azrul_qld@iium.edu.my</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
   <si>
     <t>MOU</t>
@@ -192,7 +198,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial Narrow"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve">1) 3 students (Outbound credited) Sem 2, 2018/2019
 </t>
@@ -203,7 +208,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial Narrow"/>
-        <family val="2"/>
       </rPr>
       <t>January - June 2022</t>
     </r>
@@ -212,10 +216,19 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial Narrow"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - No activity reported</t>
     </r>
+  </si>
+  <si>
+    <t>Dr. Mohd Azrul Azlen bin Abd Hamid
+Kulliyyah of Languages and Management
+International Islamic University Malaysia (IIUM) Pagoh Edu Hub
+KM 1, Jalan Panchor,
+84600, Pagoh, Muar,
+Johor Darul Takzim,
+Tel : 06 - 974 2606
+Email : azrul_qld@iium.edu.my</t>
   </si>
   <si>
     <t>Expired</t>
@@ -238,7 +251,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial Narrow"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve">1) 10 students join research presentation (Outbound non credited) Sem 1, 2018/2019
 2) 3 exchange students ( Inbound credited) Sem 1, 2019/2020
@@ -250,7 +262,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial Narrow"/>
-        <family val="2"/>
       </rPr>
       <t>January - June 2022</t>
     </r>
@@ -259,7 +270,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial Narrow"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> -  No activity reported
 </t>
@@ -270,7 +280,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial Narrow"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve">July - December 2022 - </t>
     </r>
@@ -279,50 +288,865 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial Narrow"/>
-        <family val="2"/>
       </rPr>
       <t>No activity reported</t>
     </r>
   </si>
   <si>
-    <t>Assoc. Prof. Dr. Mohd Azrul Azlen bin Abd Hamid|
-Kulliyyah of Languages and Management|
+    <t>Student Exchange Agreement</t>
+  </si>
+  <si>
+    <t>Universiti Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>Brunei</t>
+  </si>
+  <si>
+    <t>Exchange of students</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">1) 3 exchange students (Inbound credited) on Sem 1, 2017/2018
+2) 2 exchange students (Inbound credited) on Sem 2, 2018/2019
+3) 11 students (Outbound credited) on Sem 2, 2019/2020
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">January - June 2022 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">No activity reported
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">July - December 2022 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">No activity reported
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>Jan - June 2023</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve"> - No activity reported</t>
+    </r>
+  </si>
+  <si>
+    <t>Majlis Agama Islam Dan Istiadat Melayu Perlis (MAIPS)</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>1. Propose to appoint a scholar with the rank of professor or associate professor who specializes in the study of As-Sunnah as the incumbent of the Jamalullail Chair;
+ 2. Promote and advertise the Jamalullail Chair to the public;
+ 3. Select fifty (50) Doctoral students as decided and approved by the Joint Committee;
+ 4. Organize International Seminar Series and Lecture Series related to studies conducted in collaboration with IIUM and MAIPs and subject to approval at MAIPs level;
+ 5. Publish joint scholarly works to provide understanding and awareness of holistic Islamic education and meet current demands as well as subject to approval at the MAIPs level;
+ 6. Recommend to MAIPs the terms and references of appointment of the incumbent of the Chair;
+ 7. Submit annual expenditure reports to MAIPs; and
+ 8. Prepare and submit staged reports not later than the 7th of each month to MAIPs or at any time required by MAIPs.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">January - June 2022 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">1) 1st University In Action Symposium on 17 June 2022 at IIUM Gallery, Gombak
+2) Title of research : Opening of Jamalullail Responsible Research Grants
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>July - December 2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve"> - No activity reported
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>Jan - June 2023</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve"> - No activity reported</t>
+    </r>
+  </si>
+  <si>
+    <t>Ministry of Education (Institute of Teacher Education Malaysia)</t>
+  </si>
+  <si>
+    <t>1) Conference
+2) Training
+3) Research
+4) Publication
+5) Innovation
+6) Post Graduate Studies Other Related Field</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">1) International Language and Tourism Conference (ILTC), ICLET 2021 on 28 June 2021
+2) International Research Journal of Education and Sciences (IRJES) on 25 June 2022 at Royale Borneo Hotel, Tawau Sabah
+3) Research : Kerancuan Bahasa Dalam Filem Kl Gangster: Suatu Analisis Linguistik Berdasarkan Tahap 4 Kemahiran Bertutur Kerangka Standard Bahasa Melayu (KSBM)
+4) Title of publication: Antologi Satu Hari Satu Cerita-PLC Tinta Kreatif
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>July-Dec 2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">
+5) Appointment as editor for Jurnal Pendidikan Teknokrat II, Technic Education Campus Teachers Training Institut, Bandar Enstek Nilai, Ministry of Education Malaysia from 2022 until 2023 effective 17th June 2022 ( Associate Professor Dr Faridah binti Nazir)
+6)  Appointment as editor for Jurnal Refleksi Kepimpinan,Technic Education Campus Teachers Training Institute, Bandar Enstek, Nilai, Ministry of Education Malaysia editor from 2022 until 2023 effective 17th June 2022. (Associate Professor Dr Faridah binti Nazir)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>Publication</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">
+7) “Sepandai-pandai tupai melompat, akhirnya jatuh ke tanah juga”. Cerita Pendek, Satu Hari Satu Cerita:Pupuklah Jiwa. Seremban, Negeri Sembilan: Institut Pendidikan Guru Kampus Raja Melewar.
+8) Sajak “Milik Kita”. Antologi Puisi Kanak-Kanak Rimbunan Kasih.  Seremban, Negeri Sembilan: Institut Pendidikan Guru Kampus Raja Melewar.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>Jan - June 2023</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve"> - No activity reported</t>
+    </r>
+  </si>
+  <si>
+    <t>Associate Professor Dr Faridah binti Nazir
+Department of Malay for International Communication
+Kulliyyah of Languages and Management
 International Islamic University Malaysia (IIUM) Pagoh Edu Hub
 KM 1, Jalan Panchor,
 84600, Pagoh, Muar,
-Johor Darul Takzim,|
-06 - 974 2606|
-azrul_qld@iium.edu.my</t>
-  </si>
-  <si>
-    <t>Dr. Mohd Azrul Azlen bin Abd Hamid|
-Kulliyyah of Languages and Management|
-International Islamic University Malaysia (IIUM) Pagoh Edu Hub
-KM 1, Jalan Panchor,
-84600, Pagoh, Muar,
-Johor Darul Takzim,|
-06 - 974 2606|
-azrul_qld@iium.edu.my</t>
-  </si>
-  <si>
-    <t>Dr. Mohd Azrul Azlen bin Abd Hamid|
-Kulliyyah of Languages and Management|
-International Islamic University Malaysia (IIUM) Pagoh Edu Hub
-KM 1, Jalan Panchor,
-84600, Pagoh, Muar,
-Johor Darul Takzim,|
- 06 - 974 2606|
-azrul_qld@iium.edu.my|</t>
-  </si>
-  <si>
-    <t>Active</t>
+Johor Darul Takzim,
+Email: fidafn@iium.edu.my</t>
+  </si>
+  <si>
+    <t>MOU &amp; SEA</t>
+  </si>
+  <si>
+    <t>Doshisha University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(a)   Exchange of faculty;
+(b)   Exchange of students;
+(c)    Joint research projects;
+(d)    Joint seminars and conferences;
+(e)    Exchange of research materials and resources; and
+(f)     Any other areas of co-operation to be mutually agreed upon by the Parties.
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">1) 2 exchange students (Outbound credited) Sem 2, 2014/2015                                
+2) 1 exchange student (Inbound credited) Sem 1, 2015/2016                                                                
+3) 1 exchange student (Outbound credited) Sem 2, 2015/2016
+4) 2 exchange students (Outbound credited) Sem 1, 2016/2017.                    
+5) 3 exchange students (Outbound credited) Sem 1, 2017/2018.   
+6) 3 exchange students (Outbound credited) Sem 2, 2018/2019  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>January - June 2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve"> - No activitiy reported
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>July - Dec 2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">
+1) 2 exchange students (Outbound credited) Sem 1, 2022/2023
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>Jan - June 2023</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve"> - No activity reported</t>
+    </r>
+  </si>
+  <si>
+    <t>University Echahid Hamma Lakhdar El-Oued</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>(a) Student mobility – activities may include:
+ i. Exchange of undergraduate and graduate students;
+ ii. Facilitate the admission of undergraduate and graduate students;
+ iii. Visiting students’ program;
+ iv. Summer school;
+ v. Study-abroad programs;
+ vi. Language training; and
+ vii. Internships.
+ (b) Joint programs – activities may include:
+ i. Collaborative training of undergraduate and graduate
+ students through joint academic programs (including dual-degree programs); and
+ ii. Co-supervision of doctoral theses (cotutelle).
+ (c) Knowledge transfer – activities may include:
+ i. Exchange of publications and other academic materials;
+ ii. Exchange of faculty members for teaching; and
+ iii. Conferences, workshops and seminars.
+ (d) Research collaborations – activities may include:
+ i. Exchange of faculty members, graduate students and postdoctoral fellows;
+ ii. Development of joint research projects and programs; and
+ iii. Collaborative scholarly publications.
+ (e) any other areas of co-operation to be mutually agreed upon by the Parties.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">1) 15 students (Inbound credited) on Sem 1, 2018/2019
+2) 4 students (Outbound credited) on Sem 1,2018/2019
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>July - December 2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve"> - No activity reported
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>Jan - June 2023</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve"> - No activity reported</t>
+    </r>
+  </si>
+  <si>
+    <t>Asst. Prof. Dr. Nur Hidayah Abd Rahman
+Department of Tourism Planning and Hospitality Management,
+Kulliyyah of Languages and Management,
+International Islamic University Malaysia, Pagoh Campus
+Email: hidayah_rahman@iium.edu.my</t>
+  </si>
+  <si>
+    <t>BH Travel Sdn Bhd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(a) To have student internship program and staff’s attachment under the supervision of both parties (local or oversea). To exchange of information, resources, promotional and scholarly communication.
+(b) To have discussion on sustainable tourism issues and planning with associations, professional bodies and local or international corporate companies. 
+(c) Other areas of cooperation including conducting specific short courses as and when possible: 
+i. Umrah &amp; hajj enhancement course; 
+ii. banteraharmoni - Mosque, madrasah and Islamic activities centre enhancement courses; 
+iii. bantuhijau – Planned program designed to promote the adoption of green technologies and to perform green practices.
+iv. Any other areas of co-operation to be mutually agreed upon by the Parties. 
+</t>
+  </si>
+  <si>
+    <t>No activity reported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr Samshul Amry bin Abdul Latif 
+Kulliyyah of Languages and Management, 
+Pagoh Edu Hub, KM1, Jalan Panchor 84600 
+Pagoh, Muar, Johor Darul Takzim
+Tel: 06-9742766 
+Email: iium_samshul@iium.edu.my 
+</t>
+  </si>
+  <si>
+    <t>Syria Care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(a) Knowledge Transfer Project (KTP). The activities may include:
+● Organizing online language classes; and
+● Sharing session on volunteerism and humanitarian activities.
+(b) Joint programs:
+● Entrepreneurship training(s); and
+● Volunteering activities organize by Syria Care.
+(c) Encouraging the staff to waqf their time for all volunteering activities.
+(d) any other areas of co-operation to be mutually agreed upon by the Parties.
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">Jan - June 2022
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">Syria Care 13.0 humanitarian mission to Lebanon dari 11 April - 19 April 2022
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">July -Dec 2022
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>Kempen Bantuan Musim Sejuk 10.0 on 23 Oct 2022</t>
+    </r>
+  </si>
+  <si>
+    <t>Fukushima University</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>Jan - June 2023</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve"> - No activity reported</t>
+    </r>
+  </si>
+  <si>
+    <t>Embassy of France and Association Malaisienne des Professeurs de Francais</t>
+  </si>
+  <si>
+    <t>1) To conduct a French Language Day for IIUM students to enhance their skills and knowledge on the French Language through exhibition and competition
+2) To establish a media library on the Franch Language to IIUM students
+3) To conduct 1 day training on the Franch Civilization and regional culture and
+4) To acknowledge the financial support from the EoF and AMPF in any of its publications, marketing and/or publicity initiatives related to the project.</t>
+  </si>
+  <si>
+    <t>Urgench State University</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(a)        Student mobility – activities may include:
+i.    Exchange of undergraduate and graduate students;
+ii.    Facilitate the admission of undergraduate and graduate students;
+iii.   Visiting students’ program;
+iv.   Summer school;
+v.    Study-abroad programs;
+vi.   Language training; and
+vii.  Internships.
+(b)        Joint programs – activities may include:
+i.      Collaborative training of undergraduate and graduate
+students through joint academic programs (including dual-degree programs); and
+ii.      Co-supervision of doctoral theses (cotutelle).
+(c)        Knowledge transfer – activities may include:
+i.      Exchange of publications and other academic materials;
+ii.     Exchange of faculty members for teaching; and
+iii.    Conferences, workshops and seminars.
+(d)        Research collaborations – activities may include:
+i.       Exchange of faculty members, graduate students and postdoctoral fellows;
+ii.       Development of joint research projects and programs; and
+iii.      Collaborative scholarly publications.
+(e)        any other areas of co-operation to be mutually agreed upon by the Parties.
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">Jan - June 2022
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">1) Title of Publication: Travel Motivations and Travel Careers of Malaysian Backpackers
+2) IIUM-UrSU Lecture Series: Malaysia's Marketing Strategies for Domestic Tourism (Part 1) on 9 June 2022 thru online platform
+3) Online Sharing session with Guest Lecturer from Urgench State University on 16 May 2022
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">July - Dec 2022
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">1) Online class for topic Marketing Distribution in Tourism by Guest Lecturer from Urgench State University on 14 December 2022. Attended by 23 students.
+2) Title of publication: Travel Motivations and Travel Careers of Malaysian Backpackers
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>Jan - June 2023</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve"> - No activity reported</t>
+    </r>
+  </si>
+  <si>
+    <t>Asst. Prof. Dr. Samshul Amry Abdul Latif
+Kulliyyah of Languages and Management,
+International Islamic University Malaysia, Pagoh Campus
+Email: iium_samshul@iium.edu.my
+Tel : 069742708</t>
+  </si>
+  <si>
+    <t>Universitas Pendidikan Indonesia</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(a)	Promotion of joint research;
+(b)	Exchange of undergraduate and postgraduate students;
+(c)	Exchange of faculty members and administrative staffs;
+(d)	Exchange of research outcomes, academic publications, and other academic information;
+(e)	any other areas of co-operation to be mutually agreed upon by the Parties.
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>July -Dec 2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">
+1) 13 students (Inbound credited) Sem 1, 2022/2023
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>Jan - June 2023</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve"> - No activity reported</t>
+    </r>
+  </si>
+  <si>
+    <t>Guizhou Minzu University</t>
+  </si>
+  <si>
+    <t>(a)   Student and staff exchange and mobility – activities may include:
+       i.    Facilitate the admission of undergraduate and graduate students;
+       ii.   Facilitate staff attachment
+       iii.   Language training
+       iv.   Visiting students' program; and
+       v.   Internships.
+(b)   Joint programs – activities may include:
+        i.     Facilitate online courses, workshops, webinars, and conferences; 
+        ii.    Collaborative research, lecture, discussions and training of professors and researchers.
+(c)    Research and innovation; and
+(d)    any other areas of co-operation to be mutually agreed upon by the Parties.</t>
+  </si>
+  <si>
+    <t>Asst. Prof. Dr. Siti Yuliandi binti Ahmad
+Kulliyyah of Languages and Management
+International Islamic University Malaysia
+Pagoh Edu Hub, Johor
+Email: sitiyuliandi@iium.edu.my
+Tel: 069742602</t>
+  </si>
+  <si>
+    <t>Sun Moon University</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(a)   Student and staff exchange and mobility – activities may include:
+       i.    Facilitate the admission of undergraduate and graduate students;
+       ii.   Credit transfer;
+       iii.   Visiting lectures and students' program; and
+       iv.   Internships.
+(b)   Joint programs – activities may include:
+        i.     Facilitate online courses, workshops, webinars, and conferences; 
+        ii.    Joint students activities;
+        iii.    Collaborative research, lecture, discussions and training of professors and researchers.
+(c)    Research and innovation; and
+(d)    any other areas of co-operation to be mutually agreed upon by the Parties.
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve">1)   64 students (Inbound non-credited) for Summer Camp 2011
+2)   39 students (inbound credited) in 2013.
+3)   6 students (Outbound) Sem 2, 2014/2015
+4)   5 students (Inbound) Sem 1, 2015/2016
+5)   3 students (Inbound) Sem 1, 2016/2017 
+6)   8 students (Outbound) Sem 1, 2016/2017
+7)   6 students (Inbound) Sem 1, 2017/2018
+8)   7 students (Outbound) Sem 1,2017/2018
+9)   3 Students (Inbound) Sem 2, 2017/2018
+10) 1 student (Outbound) Sem 2, 2017/2018
+11) 2 students (Inbound) Sem 1, 2018/2019
+12) 5 students (Outbound) Sem 1, 2018/2019
+13) 2 students (outbound credited) Sem 1, 2022/2023
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t>Jan - June 2023</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+      </rPr>
+      <t xml:space="preserve"> - 3 students exchange (Outbound credited) Sem 2, 2022/2023</t>
+    </r>
+  </si>
+  <si>
+    <t>Universitas Ahmad Dahlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(a)	Academic partnerships;
+Academic partnerships-Joint programs which include activities:
+i.	Facilitate online courses, workshops, webinars, and conferences; 
+ii.	Joint students activities;
+iii.	Collaborative research, lecture, discussions and training of professors and researchers.
+(b)	Exchange of students and staff;
+Student and staff exchange and mobility – activities may include:
+i.	Facilitate the admission of undergraduate and postgraduate students;
+ii.	Visiting lectures and students' program; and
+iii.	Internships.
+(c)	Joint research; 
+i.     Journal publication 
+ii.    Book publication 
+(d)	Any other areas of co-operation to be mutually agreed upon by the Parties.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr Arina binti Johari
+Kulliyyah of Languages and Management,
+International Islamic University Malaysia,
+Jalan Gombak,
+53100 Kuala Lumpur, Malaysia.
+Tel. No.     :+606- 974 -2602
+Email        :arinajr@iium.edu.my
+</t>
+  </si>
+  <si>
+    <t>Universiti Teknologi Mara</t>
+  </si>
+  <si>
+    <t>(a) Promotion of joint research
+(b) Exchange of undergraduate and postgraduate students
+(c) Exchange of faculty members and administrative staff
+(d) Exchange of research outcomes, academic publication and other academic information
+(e) Organizing conferences, seminars, webinars and workshops; and
+(f) any other areas of co-operation to be mutually agreed upon by the parties.</t>
+  </si>
+  <si>
+    <t>Asst. Porf. Dr. Nur Nabilah binti Abdullah
+Kulliyyah of Languiages and Management
+IIUM Pagoh Campus
+Johor
+Email: nnabilah@iium.edu.my
+Tel. no: 069741131</t>
+  </si>
+  <si>
+    <t>Shenandoah University</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Kulliyyah of Engineering, Kulliyyah of Pharmacy, Kulliyyah of Languages and Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a)	to facilitate visits by individuals from each Party for the purpose of studying the other's educational system in order to develop cooperative mechanisms and to expand areas of cooperation;
+b)	to identify other areas of possible interest and collaboration; and
+c)	and to make faculty and students aware of the academic programs, research institutes, and educational resources of each other's institutions.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prof. Dr. Mohamad Haniki Nik Mohamed
+Kulliyyah of Pharmacy
+International Islamic University Malaysia 
+Jalan Sultan Ahmad Shah, Bandar Indera Mahkota
+25200 Kuantan, Pahang
+Tel:        (609)-5704903
+Email:     haniki@iium.edu.my
+Dr. ’Atiah Abdullah Sidek
+Kulliyyah of Engineering
+International Islamic University Malaysia,
+53100 Jalan Gombak, Gombak, Selangor
+Tel:             (603)-64214579
+Email:        atiahas@iium.edu.my
+Dr. Nor Zainiyah Norita Mokhtar
+Kulliyyah of Languages and Management,
+International Islamic University Malaysia, Pagoh Education Hub, KM 1, 
+Jalan Panchor, Pagok 84600 Muar, Johor.
+Tel:        06-9742690
+Email:     mnzainiyah@iium.edu.my
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd&quot;-&quot;mmm&quot;-&quot;yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd\-mmm\-yy"/>
+  </numFmts>
+  <fonts count="16">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,7 +1158,6 @@
       <sz val="13"/>
       <color theme="1"/>
       <name val="Arial Narrow"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -347,13 +1170,11 @@
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="13"/>
       <color theme="1"/>
       <name val="Arial Narrow"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="13"/>
@@ -364,13 +1185,11 @@
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial Narrow"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -382,10 +1201,35 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial Narrow"/>
-      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;docs-Arial Narrow&quot;"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;docs-Arial Narrow&quot;"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,8 +1260,14 @@
         <bgColor theme="5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -486,103 +1336,244 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="8" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -924,24 +1915,24 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.21875" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" customWidth="1"/>
-    <col min="3" max="3" width="42.77734375" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="41" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="7" width="21.21875" customWidth="1"/>
-    <col min="8" max="8" width="22.77734375" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
     <col min="9" max="9" width="78" customWidth="1"/>
-    <col min="10" max="10" width="101.5546875" customWidth="1"/>
-    <col min="11" max="11" width="63.21875" customWidth="1"/>
+    <col min="10" max="10" width="101.5703125" customWidth="1"/>
+    <col min="11" max="11" width="63.28515625" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1005,7 +1996,7 @@
       <c r="G2" s="15">
         <v>42416</v>
       </c>
-      <c r="H2" s="31">
+      <c r="H2" s="67">
         <v>45353</v>
       </c>
       <c r="I2" s="16" t="s">
@@ -1015,10 +2006,10 @@
         <v>17</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="141.75" customHeight="1">
@@ -1026,13 +2017,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>15</v>
@@ -1047,16 +2038,16 @@
         <v>44829</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K3" s="28" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="141" customHeight="1">
@@ -1067,10 +2058,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>15</v>
@@ -1085,34 +2076,620 @@
         <v>45034</v>
       </c>
       <c r="I4" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="19" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="5" spans="1:12" ht="163.5" customHeight="1"/>
-    <row r="6" spans="1:12" ht="272.25" customHeight="1"/>
-    <row r="7" spans="1:12" ht="359.25" customHeight="1"/>
-    <row r="8" spans="1:12" ht="219.75" customHeight="1"/>
-    <row r="9" spans="1:12" ht="314.25" customHeight="1"/>
-    <row r="10" spans="1:12" ht="324" customHeight="1"/>
-    <row r="11" spans="1:12" ht="168.75" customHeight="1"/>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:12" ht="182.25" customHeight="1"/>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1"/>
-    <row r="15" spans="1:12" ht="117.75" customHeight="1"/>
-    <row r="16" spans="1:12" ht="234" customHeight="1"/>
-    <row r="17" ht="264" customHeight="1"/>
-    <row r="18" ht="280.5" customHeight="1"/>
-    <row r="19" ht="153" customHeight="1"/>
-    <row r="20" ht="387" customHeight="1"/>
+    <row r="5" spans="1:12" ht="163.5" customHeight="1">
+      <c r="A5" s="31">
+        <v>4</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="34">
+        <v>2019</v>
+      </c>
+      <c r="G5" s="35">
+        <v>43527</v>
+      </c>
+      <c r="H5" s="35">
+        <v>45353</v>
+      </c>
+      <c r="I5" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="272.25" customHeight="1">
+      <c r="A6" s="31">
+        <v>5</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="34">
+        <v>2019</v>
+      </c>
+      <c r="G6" s="35">
+        <v>43629</v>
+      </c>
+      <c r="H6" s="35">
+        <v>45455</v>
+      </c>
+      <c r="I6" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="359.25" customHeight="1">
+      <c r="A7" s="31">
+        <v>6</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="34">
+        <v>2019</v>
+      </c>
+      <c r="G7" s="35">
+        <v>43662</v>
+      </c>
+      <c r="H7" s="35">
+        <v>45488</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="219.75" customHeight="1">
+      <c r="A8" s="31">
+        <v>7</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="34">
+        <v>2020</v>
+      </c>
+      <c r="G8" s="42">
+        <v>44011</v>
+      </c>
+      <c r="H8" s="42">
+        <v>45836</v>
+      </c>
+      <c r="I8" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="314.25" customHeight="1">
+      <c r="A9" s="31">
+        <v>8</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="34">
+        <v>2020</v>
+      </c>
+      <c r="G9" s="44">
+        <v>44159</v>
+      </c>
+      <c r="H9" s="44">
+        <v>45253</v>
+      </c>
+      <c r="I9" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="324" customHeight="1">
+      <c r="A10" s="19">
+        <v>9</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="45">
+        <v>2021</v>
+      </c>
+      <c r="G10" s="24">
+        <v>44264</v>
+      </c>
+      <c r="H10" s="46">
+        <v>44993</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="168.75" customHeight="1">
+      <c r="A11" s="19">
+        <v>10</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="45">
+        <v>2021</v>
+      </c>
+      <c r="G11" s="24">
+        <v>44298</v>
+      </c>
+      <c r="H11" s="46">
+        <v>45027</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="J11" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A12" s="31">
+        <v>11</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="48">
+        <v>2021</v>
+      </c>
+      <c r="G12" s="44">
+        <v>44337</v>
+      </c>
+      <c r="H12" s="49">
+        <v>45432</v>
+      </c>
+      <c r="I12" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="182.25" customHeight="1">
+      <c r="A13" s="19">
+        <v>12</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="45">
+        <v>2021</v>
+      </c>
+      <c r="G13" s="24">
+        <v>44337</v>
+      </c>
+      <c r="H13" s="46">
+        <v>44701</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A14" s="31">
+        <v>13</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="48">
+        <v>2021</v>
+      </c>
+      <c r="G14" s="44">
+        <v>44337</v>
+      </c>
+      <c r="H14" s="49">
+        <v>45432</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="117.75" customHeight="1">
+      <c r="A15" s="31">
+        <v>14</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="31">
+        <v>2021</v>
+      </c>
+      <c r="G15" s="54">
+        <v>44533</v>
+      </c>
+      <c r="H15" s="55">
+        <v>45628</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="234" customHeight="1">
+      <c r="A16" s="31">
+        <v>15</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="58">
+        <v>2021</v>
+      </c>
+      <c r="G16" s="60">
+        <v>44530</v>
+      </c>
+      <c r="H16" s="61">
+        <v>46355</v>
+      </c>
+      <c r="I16" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="L16" s="63"/>
+    </row>
+    <row r="17" spans="1:12" ht="264" customHeight="1">
+      <c r="A17" s="31">
+        <v>16</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="31">
+        <v>2022</v>
+      </c>
+      <c r="G17" s="55">
+        <v>44623</v>
+      </c>
+      <c r="H17" s="55">
+        <v>45718</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="J17" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="280.5" customHeight="1">
+      <c r="A18" s="31">
+        <v>17</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="31">
+        <v>2023</v>
+      </c>
+      <c r="G18" s="64">
+        <v>45092</v>
+      </c>
+      <c r="H18" s="64">
+        <v>46156</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="J18" s="65" t="s">
+        <v>61</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="153" customHeight="1">
+      <c r="A19" s="31">
+        <v>18</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="31">
+        <v>2023</v>
+      </c>
+      <c r="G19" s="64">
+        <v>45134</v>
+      </c>
+      <c r="H19" s="64">
+        <v>46229</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="J19" s="66"/>
+      <c r="K19" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="387" customHeight="1">
+      <c r="A20" s="31">
+        <v>19</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="31">
+        <v>2023</v>
+      </c>
+      <c r="G20" s="64">
+        <v>45166</v>
+      </c>
+      <c r="H20" s="64">
+        <v>46261</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" s="66"/>
+      <c r="K20" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L20" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Updated: Activity management to depend on collaboration records instead of agreement records. - Updated: Activity view and delete handling. - Added: Component for creating headers of each activity record. - Added: Checker for existing collaboration records and functionality to populate them in the create form. - Updated: Log table to store changes occurring in the agreement table. - Updated: Unique agreement ID generation now based on `agreement_id_seq`. - Updated: Forms to enforce max length constraints and to empty default values. - Updated: Special agreement record functionality. - Updated: Files are now named using the format `filename_date.extension`.
</commit_message>
<xml_diff>
--- a/common/uploads/import_.xlsx
+++ b/common/uploads/import_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yamen\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABAZAZILAH\Downloads\moumoa\import files test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C96459-A2A3-4D7C-BF7B-26E33A7483BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08AC23D-51C7-47D1-93C1-14D42ED5F49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4F3D802B-CD53-4E1B-9F2D-46E99AA13B81}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4F3D802B-CD53-4E1B-9F2D-46E99AA13B81}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,15 +92,9 @@
     <t>MOU</t>
   </si>
   <si>
-    <t xml:space="preserve">	Kansai University</t>
-  </si>
-  <si>
     <t>Japan</t>
   </si>
   <si>
-    <t xml:space="preserve">	KICT</t>
-  </si>
-  <si>
     <t>Project Title Title Project</t>
   </si>
   <si>
@@ -132,6 +126,12 @@
   </si>
   <si>
     <t>Collaborator Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	 University of Kansai</t>
+  </si>
+  <si>
+    <t>KICT</t>
   </si>
 </sst>
 </file>
@@ -535,13 +535,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C8D2A1-A96E-4B71-8E3B-ADD69BF0C10B}">
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -576,7 +576,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>11</v>
@@ -597,24 +597,24 @@
         <v>16</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="F2" s="1">
         <v>1000</v>
@@ -623,28 +623,28 @@
         <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="K2" s="1">
         <v>193079894</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="P2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="Q2" s="4">
         <v>45464</v>
@@ -653,40 +653,40 @@
         <v>45940</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="26" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="mailto:%20yamen.zaiter24@gmail.com" xr:uid="{B670A1A0-A540-4CEF-AA92-A1C220AE1B70}"/>

</xml_diff>